<commit_message>
Updating ops for ball and brick messages.
</commit_message>
<xml_diff>
--- a/OpCodes.xlsx
+++ b/OpCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\NetworkedPIGMjs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{920D0728-D1A8-409C-9B35-F1D8893FF756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1629570-9E81-446F-A73B-6258D2ED3B9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1815C293-3D78-461A-A368-54D841B26A9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>SuperOp</t>
   </si>
@@ -57,13 +57,22 @@
   </si>
   <si>
     <t>Server</t>
+  </si>
+  <si>
+    <t>BallBounced</t>
+  </si>
+  <si>
+    <t>Brick hit</t>
+  </si>
+  <si>
+    <t>Brick destroyed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,16 +88,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -96,11 +124,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -108,11 +211,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A82CD3-3EFC-4802-9B8B-1AF979233DBD}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,39 +587,86 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>